<commit_message>
feat:add send message tool
</commit_message>
<xml_diff>
--- a/src/send_message/index.xlsx
+++ b/src/send_message/index.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,23 +412,31 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>郭鑫惺</v>
+        <v>QQ邮箱</v>
       </c>
       <c r="B2" t="str">
-        <v>2443760268gxx@gmail.com</v>
+        <v>1652675907@qq.com</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>杜佳文</v>
+        <v>谷歌邮箱</v>
       </c>
       <c r="B3" t="str">
-        <v>1415006080@qq.com</v>
+        <v>pitousanfadetuzi@gmail.com</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>网易邮箱</v>
+      </c>
+      <c r="B4" t="str">
+        <v>13376003432@163.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>